<commit_message>
modification de la doc
</commit_message>
<xml_diff>
--- a/journal_de_travail.xlsx
+++ b/journal_de_travail.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\1re année\Modules I-CT\ICT-431&amp;MA-20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\1re année\Modules I-CT\ICT-431&amp;MA-20\2048_0.3.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>date</t>
   </si>
@@ -108,6 +108,24 @@
   </si>
   <si>
     <t>résolution de bug</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>ajout d'une option de réinitialisation du meilleur score et résolution de bug</t>
+  </si>
+  <si>
+    <t>une grande partie du temps a été consacrée à rendre le projet</t>
+  </si>
+  <si>
+    <t>optimisation du code, résolution d'un bug de fenêtre et ajout de la victoire</t>
+  </si>
+  <si>
+    <t>fin des sprint sur icecrum</t>
+  </si>
+  <si>
+    <t>Aider Théo pour sa fonction de défaite</t>
   </si>
 </sst>
 </file>
@@ -277,8 +295,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -553,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +651,7 @@
     <col min="5" max="5" width="11.42578125" style="7"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="39.85546875" style="24" customWidth="1"/>
-    <col min="8" max="8" width="37" customWidth="1"/>
+    <col min="8" max="8" width="37" style="24" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -593,7 +677,7 @@
       <c r="G1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="22" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="21" t="s">
@@ -623,7 +707,7 @@
       <c r="G2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -640,7 +724,7 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E33" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E34" si="0">D3-C3</f>
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -649,7 +733,7 @@
       <c r="G3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
@@ -677,7 +761,7 @@
       <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -703,7 +787,7 @@
       <c r="G5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -729,7 +813,7 @@
       <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -755,7 +839,7 @@
       <c r="G7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -781,7 +865,7 @@
       <c r="G8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -807,7 +891,7 @@
       <c r="G9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -833,7 +917,7 @@
       <c r="G10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -859,7 +943,7 @@
       <c r="G11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="10" t="s">
         <v>22</v>
       </c>
       <c r="I11" s="1"/>
@@ -887,7 +971,7 @@
       <c r="G12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -913,7 +997,7 @@
       <c r="G13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="1"/>
@@ -941,7 +1025,7 @@
       <c r="G14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="10"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -967,77 +1051,139 @@
       <c r="G15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>45002</v>
+      </c>
+      <c r="B16" s="8">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.50694444444444442</v>
+      </c>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="1"/>
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="4">
+        <v>45009</v>
+      </c>
+      <c r="B17" s="8">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.37847222222222227</v>
+      </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="1"/>
+        <v>3.4722222222222654E-3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="10"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45009</v>
+      </c>
+      <c r="B18" s="8">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="10"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="4">
+        <v>45009</v>
+      </c>
+      <c r="B19" s="8">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.46666666666666662</v>
+      </c>
       <c r="E19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="1"/>
+        <v>8.3333333333333037E-3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="10"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="4">
+        <v>45009</v>
+      </c>
+      <c r="B20" s="8">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.4826388888888889</v>
+      </c>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="1"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="10"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1051,7 +1197,7 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1065,7 +1211,7 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1079,7 +1225,7 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1093,7 +1239,7 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="1"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1107,7 +1253,7 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1121,7 +1267,7 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1135,7 +1281,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1149,7 +1295,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="1"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1163,7 +1309,7 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="1"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1177,7 +1323,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="1"/>
+      <c r="H30" s="10"/>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1191,7 +1337,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="1"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,7 +1351,7 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1219,10 +1365,53 @@
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="1"/>
+      <c r="H33" s="10"/>
       <c r="I33" s="1"/>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="7">
+        <f>SUM(E2:E34)</f>
+        <v>0.9437500000000002</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="admin">
+      <formula>NOT(ISERROR(SEARCH("admin",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="rien">
+      <formula>NOT(ISERROR(SEARCH("rien",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="autre">
+      <formula>NOT(ISERROR(SEARCH("autre",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="aide">
+      <formula>NOT(ISERROR(SEARCH("aide",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="doc">
+      <formula>NOT(ISERROR(SEARCH("doc",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="code">
+      <formula>NOT(ISERROR(SEARCH("code",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
       <formula1>"code,doc,rien,admin,aide,autre"</formula1>

</xml_diff>